<commit_message>
[VM:timothy.queen@7/9/2014 12:21:54 PM] updated
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13635
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
+++ b/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="48" yWindow="2964" windowWidth="18900" windowHeight="4872" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="48" yWindow="2964" windowWidth="18900" windowHeight="4872" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Velocity Size Defs" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="113">
   <si>
     <t xml:space="preserve">Priority   </t>
   </si>
@@ -274,6 +274,111 @@
   <si>
     <t>Tim Queen</t>
   </si>
+  <si>
+    <t xml:space="preserve">Quantitative Priority   </t>
+  </si>
+  <si>
+    <t>P12846: eCL: Historical data that cannot match LAN ID for CSR &amp; Submitter has issues</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P12857: IQS - eCL Error Report not displaying errors from Verint feed </t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Lex</t>
+  </si>
+  <si>
+    <t>P12877: IQS/eCL/Scorecard - download of scorecard file to match on date</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>P12897: eCL - Coaching Source request</t>
+  </si>
+  <si>
+    <t>Susmiitha</t>
+  </si>
+  <si>
+    <t>P12905: eCL - Inactivations Database task</t>
+  </si>
+  <si>
+    <t>P12922 0 IQS/eCL - Database missing eval ids from GDIT Data Feed files</t>
+  </si>
+  <si>
+    <t>Pending Dev</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Suzy</t>
+  </si>
+  <si>
+    <t>P12923: eCL - Inactivations need to inactive records prior to May 5th</t>
+  </si>
+  <si>
+    <t>P12924: eCL - IQS update filter of records to send</t>
+  </si>
+  <si>
+    <t>Doug, Dave</t>
+  </si>
+  <si>
+    <t>P12926: eCL - Admin task to remove duplicate records</t>
+  </si>
+  <si>
+    <t>P12930: eCoaching Log - Display Verint scorecard name on eCL forms</t>
+  </si>
+  <si>
+    <t>Jourdain, Suzy</t>
+  </si>
+  <si>
+    <t>P12957: eCoaching - Update procedure to set EmailSent flag to True on Notifications sent</t>
+  </si>
+  <si>
+    <t>P12962: CCO eCoaching - coaching log inactivations for week of 6/23/14</t>
+  </si>
+  <si>
+    <t>Pending info</t>
+  </si>
+  <si>
+    <t>P12963: eCL - Quality Filelist count loaded updated incorrectly</t>
+  </si>
+  <si>
+    <t>implement</t>
+  </si>
+  <si>
+    <t>P12978: eCoaching - Update eCL Access Control Application to point to new eCoaching database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jourdain  </t>
+  </si>
+  <si>
+    <t>P12982: CCO eCoaching - Update employee hierarchy Load process</t>
+  </si>
+  <si>
+    <t>V&amp;V</t>
+  </si>
+  <si>
+    <t>P12983: CCO Coaching - review &amp; update employee id to lanid table maintenance</t>
+  </si>
+  <si>
+    <t>P13054: IQS/eCL - Added Scorecard form name to data feed</t>
+  </si>
+  <si>
+    <t>Suzy, Dave</t>
+  </si>
+  <si>
+    <t>P13071: CCO eCoaching - Create indexes and stats on eCoaching Database tables</t>
+  </si>
+  <si>
+    <t>Suzy, Doug</t>
+  </si>
 </sst>
 </file>
 
@@ -283,7 +388,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -328,6 +433,13 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -520,10 +632,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -693,8 +806,10 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2547,10 +2662,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F44" sqref="F44"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3:E5"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2650,7 +2765,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>49</v>
@@ -2678,8 +2793,8 @@
         <v>1</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>54</v>
+      <c r="F4" s="71" t="s">
+        <v>91</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>49</v>
@@ -2709,7 +2824,7 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>50</v>
@@ -2772,30 +2887,46 @@
       <c r="O8" s="43"/>
     </row>
     <row r="9" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
+      <c r="A9" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="2"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="18"/>
+      <c r="N9" s="18">
+        <v>41821</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
+      <c r="A10" s="50" t="s">
+        <v>111</v>
+      </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="2"/>
       <c r="M10" s="15"/>
-      <c r="N10" s="18"/>
+      <c r="N10" s="18">
+        <v>41822</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="55"/>
@@ -3765,24 +3896,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F44" sqref="F44"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.5546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="9.109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="12.109375" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
@@ -3803,8 +3935,8 @@
       <c r="B1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>0</v>
+      <c r="C1" s="26" t="s">
+        <v>78</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>5</v>
@@ -4002,10 +4134,14 @@
       <c r="N8" s="42"/>
       <c r="O8" s="43"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
+    <row r="9" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="2"/>
       <c r="F9" s="1"/>
@@ -4013,276 +4149,424 @@
       <c r="J9" s="4"/>
       <c r="K9" s="2"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="18"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
+      <c r="N9" s="18">
+        <v>41800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
       <c r="J10" s="4"/>
       <c r="K10" s="2"/>
       <c r="M10" s="15"/>
-      <c r="N10" s="18"/>
-    </row>
-    <row r="11" spans="1:15" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="25" t="s">
+      <c r="N10" s="18">
+        <v>41802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6">
         <v>2</v>
       </c>
-      <c r="L11" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" s="18"/>
-    </row>
-    <row r="12" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
+      <c r="E11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>7</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="18">
+        <v>41802</v>
+      </c>
+      <c r="O11" s="17">
+        <v>41820</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="2"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="18">
+        <v>41802</v>
+      </c>
+      <c r="O12" s="17">
+        <v>41820</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
+      <c r="A13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>76</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="2"/>
       <c r="M13" s="15"/>
-      <c r="N13" s="18"/>
+      <c r="N13" s="18">
+        <v>41803</v>
+      </c>
+      <c r="O13" s="17">
+        <v>41820</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
+      <c r="A14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>76</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D14" s="6"/>
       <c r="E14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="2"/>
       <c r="J14" s="4"/>
       <c r="K14" s="2"/>
       <c r="M14" s="15"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="5">
-        <v>3</v>
-      </c>
+      <c r="N14" s="18">
+        <v>41806</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
-        <v>76</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D15" s="6"/>
       <c r="E15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="G15" s="2" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="2"/>
       <c r="M15" s="15"/>
-      <c r="N15" s="18"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="1"/>
+      <c r="N15" s="18">
+        <v>41807</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="J16" s="4"/>
       <c r="K16" s="2"/>
       <c r="M16" s="15"/>
-      <c r="N16" s="18"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
+      <c r="N16" s="18">
+        <v>41807</v>
+      </c>
+      <c r="O16" s="17">
+        <v>41816</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="2"/>
       <c r="M17" s="15"/>
-      <c r="N17" s="18"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="1"/>
+      <c r="N17" s="18">
+        <v>41808</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="J18" s="4"/>
       <c r="K18" s="2"/>
       <c r="M18" s="15"/>
-      <c r="N18" s="18"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
+      <c r="N18" s="18">
+        <v>41808</v>
+      </c>
+      <c r="O18" s="17">
+        <v>41813</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="J19" s="4"/>
       <c r="K19" s="2"/>
       <c r="M19" s="15"/>
-      <c r="N19" s="18"/>
-    </row>
-    <row r="20" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="55"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="1"/>
+      <c r="N19" s="18">
+        <v>41808</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="J20" s="4"/>
       <c r="K20" s="2"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="18"/>
-    </row>
-    <row r="21" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
+      <c r="N20" s="18">
+        <v>41809</v>
+      </c>
+      <c r="O20" s="17">
+        <v>41813</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="2"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="K21" s="2"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="18"/>
-    </row>
-    <row r="22" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5"/>
+      <c r="N21" s="18">
+        <v>41813</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="2"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J22" s="4"/>
       <c r="K22" s="2"/>
       <c r="M22" s="15"/>
-      <c r="N22" s="18"/>
-    </row>
-    <row r="23" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2"/>
+      <c r="N22" s="18">
+        <v>41813</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="K23" s="2"/>
       <c r="M23" s="15"/>
-      <c r="N23" s="18"/>
-    </row>
-    <row r="24" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5"/>
+      <c r="N23" s="18">
+        <v>41813</v>
+      </c>
+      <c r="O23" s="17">
+        <v>41820</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="1"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="J24" s="4"/>
       <c r="K24" s="2"/>
       <c r="M24" s="15"/>
-      <c r="N24" s="18"/>
-    </row>
-    <row r="25" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="5"/>
+      <c r="N24" s="18">
+        <v>41804</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="2"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J25" s="4"/>
       <c r="K25" s="2"/>
       <c r="M25" s="15"/>
-      <c r="N25" s="18"/>
-    </row>
-    <row r="26" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="5"/>
+      <c r="N25" s="18">
+        <v>41814</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="55"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="2"/>
       <c r="F26" s="1"/>
       <c r="G26" s="2"/>
@@ -4291,67 +4575,138 @@
       <c r="M26" s="15"/>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="2"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="2"/>
-      <c r="M27" s="15"/>
+    <row r="27" spans="1:15" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="25" t="s">
+        <v>48</v>
+      </c>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="2"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="2"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="18"/>
-    </row>
-    <row r="29" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="2"/>
+    <row r="28" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="63"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="69"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="J29" s="4"/>
       <c r="K29" s="2"/>
       <c r="M29" s="15"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="2"/>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="J30" s="4"/>
       <c r="K30" s="2"/>
       <c r="M30" s="15"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="E31" s="2"/>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="5">
+        <v>3</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="J31" s="4"/>
       <c r="K31" s="2"/>
       <c r="M31" s="15"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
@@ -4363,7 +4718,7 @@
       <c r="M32" s="15"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="55"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -4375,8 +4730,8 @@
       <c r="M33" s="15"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="56"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="E34" s="2"/>
@@ -4387,8 +4742,8 @@
       <c r="M34" s="15"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
       <c r="E35" s="2"/>
@@ -4424,7 +4779,7 @@
       <c r="N37" s="18"/>
     </row>
     <row r="38" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
       <c r="E38" s="2"/>
@@ -4436,7 +4791,7 @@
       <c r="N38" s="18"/>
     </row>
     <row r="39" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
+      <c r="A39" s="54"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
       <c r="E39" s="2"/>
@@ -4448,7 +4803,7 @@
       <c r="N39" s="18"/>
     </row>
     <row r="40" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="55"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
       <c r="E40" s="2"/>
@@ -4460,7 +4815,7 @@
       <c r="N40" s="18"/>
     </row>
     <row r="41" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="55"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
       <c r="E41" s="2"/>
@@ -4508,7 +4863,7 @@
       <c r="N44" s="18"/>
     </row>
     <row r="45" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+      <c r="A45" s="54"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
       <c r="E45" s="2"/>
@@ -4520,7 +4875,7 @@
       <c r="N45" s="18"/>
     </row>
     <row r="46" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
+      <c r="A46" s="55"/>
       <c r="B46" s="5"/>
       <c r="C46" s="6"/>
       <c r="E46" s="2"/>
@@ -4532,7 +4887,7 @@
       <c r="N46" s="18"/>
     </row>
     <row r="47" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
+      <c r="A47" s="55"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
       <c r="E47" s="2"/>
@@ -4544,7 +4899,7 @@
       <c r="N47" s="18"/>
     </row>
     <row r="48" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
+      <c r="A48" s="55"/>
       <c r="B48" s="5"/>
       <c r="C48" s="6"/>
       <c r="E48" s="2"/>
@@ -4555,8 +4910,8 @@
       <c r="M48" s="15"/>
       <c r="N48" s="18"/>
     </row>
-    <row r="49" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
+    <row r="49" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="55"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
       <c r="E49" s="2"/>
@@ -4567,287 +4922,479 @@
       <c r="M49" s="15"/>
       <c r="N49" s="18"/>
     </row>
-    <row r="50" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
       <c r="E50" s="2"/>
       <c r="F50" s="1"/>
       <c r="G50" s="2"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="2"/>
-    </row>
-    <row r="51" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="38"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="42"/>
-      <c r="O51" s="43"/>
-    </row>
-    <row r="52" spans="1:15" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="2"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="18"/>
+    </row>
+    <row r="51" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="54"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="6"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="2"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="2"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="18"/>
+    </row>
+    <row r="52" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="55"/>
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="1"/>
+      <c r="E52" s="2"/>
       <c r="F52" s="1"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52"/>
-      <c r="K52" s="1"/>
-      <c r="L52"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="2"/>
       <c r="M52" s="15"/>
       <c r="N52" s="18"/>
-      <c r="O52" s="18"/>
-    </row>
-    <row r="53" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="5"/>
-      <c r="E53" s="1"/>
+      <c r="C53" s="6"/>
+      <c r="E53" s="2"/>
       <c r="F53" s="1"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="16"/>
-      <c r="M53" s="2"/>
-    </row>
-    <row r="54" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="2"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="18"/>
+    </row>
+    <row r="54" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="54"/>
       <c r="B54" s="5"/>
       <c r="C54" s="6"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="1"/>
       <c r="G54" s="2"/>
-      <c r="K54" s="1"/>
-      <c r="M54" s="2"/>
-    </row>
-    <row r="55" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="2"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="18"/>
+    </row>
+    <row r="55" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="55"/>
       <c r="B55" s="5"/>
       <c r="C55" s="6"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="1"/>
       <c r="G55" s="2"/>
-      <c r="K55" s="1"/>
-      <c r="M55" s="2"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="2"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="18"/>
+    </row>
+    <row r="56" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="55"/>
       <c r="B56" s="5"/>
       <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="1"/>
+      <c r="E56" s="2"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="M56" s="2"/>
-    </row>
-    <row r="57" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="46"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="47"/>
-      <c r="I57" s="47"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="48"/>
-      <c r="M57" s="45"/>
-      <c r="N57" s="49"/>
-      <c r="O57" s="49"/>
-    </row>
-    <row r="58" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G56" s="2"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="2"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="18"/>
+    </row>
+    <row r="57" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="6"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="2"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="2"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="18"/>
+    </row>
+    <row r="58" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="B58" s="6"/>
+      <c r="B58" s="5"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="1"/>
+      <c r="E58" s="2"/>
       <c r="F58" s="1"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="6"/>
-      <c r="M58" s="1"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J58" s="4"/>
+      <c r="K58" s="2"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="18"/>
+    </row>
+    <row r="59" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
-      <c r="B59" s="6"/>
+      <c r="B59" s="5"/>
       <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="1"/>
+      <c r="E59" s="2"/>
       <c r="F59" s="1"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="6"/>
-      <c r="M59" s="2"/>
-    </row>
-    <row r="60" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J59" s="4"/>
+      <c r="K59" s="2"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="18"/>
+    </row>
+    <row r="60" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
-      <c r="B60" s="6"/>
+      <c r="B60" s="5"/>
       <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="1"/>
+      <c r="E60" s="2"/>
       <c r="F60" s="1"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="6"/>
       <c r="J60" s="4"/>
-      <c r="M60" s="2"/>
-    </row>
-    <row r="61" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="2"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="18"/>
+    </row>
+    <row r="61" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="6"/>
+      <c r="B61" s="5"/>
       <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="1"/>
+      <c r="E61" s="2"/>
       <c r="F61" s="1"/>
       <c r="G61" s="2"/>
-      <c r="M61" s="2"/>
-    </row>
-    <row r="62" spans="1:15" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J61" s="4"/>
+      <c r="K61" s="2"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="18"/>
+    </row>
+    <row r="62" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
-      <c r="B62" s="6"/>
+      <c r="B62" s="5"/>
       <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="1"/>
+      <c r="E62" s="2"/>
       <c r="F62" s="1"/>
       <c r="G62" s="2"/>
-      <c r="M62" s="2"/>
-    </row>
-    <row r="63" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J62" s="4"/>
+      <c r="K62" s="2"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="18"/>
+    </row>
+    <row r="63" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
-      <c r="B63" s="6"/>
+      <c r="B63" s="5"/>
       <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="1"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="6"/>
-      <c r="M63" s="1"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J63" s="4"/>
+      <c r="K63" s="2"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="18"/>
+    </row>
+    <row r="64" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="B64" s="6"/>
+      <c r="B64" s="5"/>
       <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="1"/>
+      <c r="E64" s="2"/>
       <c r="F64" s="1"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="6"/>
-      <c r="M64" s="2"/>
-    </row>
-    <row r="65" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J64" s="4"/>
+      <c r="K64" s="2"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="18"/>
+    </row>
+    <row r="65" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="5"/>
-      <c r="D65" s="6"/>
-      <c r="F65" s="2"/>
+      <c r="C65" s="6"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="1"/>
       <c r="G65" s="2"/>
-      <c r="M65" s="2"/>
-    </row>
-    <row r="66" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J65" s="4"/>
+      <c r="K65" s="2"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="18"/>
+    </row>
+    <row r="66" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="5"/>
       <c r="C66" s="6"/>
-      <c r="F66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="1"/>
       <c r="G66" s="2"/>
-      <c r="M66" s="1"/>
-    </row>
-    <row r="67" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="M67" s="2"/>
-    </row>
-    <row r="68" spans="1:13" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="16"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="38"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="41"/>
+      <c r="G67" s="41"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="39"/>
+      <c r="J67" s="40"/>
+      <c r="K67" s="40"/>
+      <c r="L67" s="40"/>
+      <c r="M67" s="41"/>
+      <c r="N67" s="42"/>
+      <c r="O67" s="43"/>
+    </row>
+    <row r="68" spans="1:15" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="5"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="7"/>
-    </row>
-    <row r="69" spans="1:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G68" s="2"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68"/>
+      <c r="K68" s="1"/>
+      <c r="L68"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="18"/>
+      <c r="O68" s="18"/>
+    </row>
+    <row r="69" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="5"/>
+      <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G69" s="2"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="16"/>
+      <c r="M69" s="2"/>
+    </row>
+    <row r="70" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="6"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="K70" s="1"/>
+      <c r="M70" s="2"/>
+    </row>
+    <row r="71" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="5"/>
       <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="F71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K71" s="1"/>
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="6"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G72" s="1"/>
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="46"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="47"/>
+      <c r="E73" s="48"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="47"/>
+      <c r="J73" s="48"/>
+      <c r="K73" s="48"/>
+      <c r="L73" s="48"/>
+      <c r="M73" s="45"/>
+      <c r="N73" s="49"/>
+      <c r="O73" s="49"/>
+    </row>
+    <row r="74" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
+      <c r="B74" s="6"/>
       <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G74" s="2"/>
+      <c r="H74" s="6"/>
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
+      <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
+      <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="2"/>
       <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="B76" s="6"/>
       <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
+      <c r="G76" s="2"/>
       <c r="H76" s="6"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J76" s="4"/>
+      <c r="M76" s="2"/>
+    </row>
+    <row r="77" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
+      <c r="B77" s="6"/>
       <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G77" s="2"/>
+      <c r="M77" s="2"/>
+    </row>
+    <row r="78" spans="1:15" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
+      <c r="B78" s="6"/>
       <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79"/>
-      <c r="B79" s="4"/>
-      <c r="E79" s="4"/>
+      <c r="M78" s="2"/>
+    </row>
+    <row r="79" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="6"/>
+      <c r="M79" s="1"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="6"/>
+      <c r="M80" s="2"/>
+    </row>
+    <row r="81" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="B81" s="5"/>
+      <c r="D81" s="6"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="M81" s="2"/>
+    </row>
+    <row r="82" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="6"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="M82" s="1"/>
+    </row>
+    <row r="83" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="M83" s="2"/>
+    </row>
+    <row r="84" spans="1:13" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="B84" s="5"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="7"/>
+    </row>
+    <row r="85" spans="1:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+      <c r="B85" s="5"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="2"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="6"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+      <c r="C90" s="6"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="C92" s="6"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="6"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+      <c r="C93" s="6"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="C94" s="6"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95"/>
+      <c r="B95" s="4"/>
+      <c r="E95" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[VM:timothy.queen@8/4/2014 10:59:14 AM] Updated as of 10:59 8/4
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13678
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
+++ b/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="600" windowWidth="18900" windowHeight="4872" activeTab="2"/>
+    <workbookView xWindow="-48" yWindow="600" windowWidth="18900" windowHeight="4872" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Velocity Size Defs" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="125">
   <si>
     <t xml:space="preserve">Priority   </t>
   </si>
@@ -393,6 +393,27 @@
   </si>
   <si>
     <t>jourdain</t>
+  </si>
+  <si>
+    <t>SCRs Submitted/carried forward</t>
+  </si>
+  <si>
+    <t>13263 - eCoaching - Update Coaching to allow other CSR job code users to submit coaching</t>
+  </si>
+  <si>
+    <t>13265 - CCO eCoaching - Group multiple Coaching reasons for ecls in dashboard display</t>
+  </si>
+  <si>
+    <t>13276 - eCoaching Log -there are several references of bcc that should be changed to cco</t>
+  </si>
+  <si>
+    <t>Phase II</t>
+  </si>
+  <si>
+    <t>Quality and Supervisor eCL</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -2514,10 +2535,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F44" sqref="F44"/>
-      <selection pane="bottomLeft" activeCell="N25" sqref="N25"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4182,10 +4203,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F44" sqref="F44"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5580,10 +5601,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F44" sqref="F44"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3:E5"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5759,27 +5780,43 @@
       <c r="K5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="K6" s="1"/>
-      <c r="M6" s="2"/>
+    <row r="6" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="43"/>
     </row>
     <row r="7" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="19">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="50" t="s">
+        <v>49</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="K7" s="1"/>
@@ -5787,7 +5824,7 @@
     </row>
     <row r="8" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="39"/>
@@ -5805,78 +5842,207 @@
       <c r="O8" s="43"/>
     </row>
     <row r="9" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
+      <c r="A9" s="73" t="s">
+        <v>78</v>
+      </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="J9" s="4"/>
+      <c r="C9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="4">
+        <v>5</v>
+      </c>
+      <c r="I9" s="71">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="18"/>
+      <c r="N9" s="18">
+        <v>41800</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
+      <c r="A10" s="73" t="s">
+        <v>80</v>
+      </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="J10" s="4"/>
+      <c r="C10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="4">
+        <v>3</v>
+      </c>
+      <c r="I10" s="72">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="J10" s="72">
+        <v>0.1423611111111111</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="M10" s="15"/>
-      <c r="N10" s="18"/>
+      <c r="N10" s="18">
+        <v>41802</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="J11" s="4"/>
+      <c r="A11" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="4">
+        <v>4</v>
+      </c>
+      <c r="I11" s="71">
+        <v>1.2569444444444444</v>
+      </c>
+      <c r="J11" s="72"/>
       <c r="K11" s="2"/>
       <c r="M11" s="15"/>
-      <c r="N11" s="18"/>
+      <c r="N11" s="18">
+        <v>41814</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
+      <c r="A12" s="73" t="s">
+        <v>119</v>
+      </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-      <c r="J12" s="4"/>
+      <c r="C12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="4">
+        <v>4</v>
+      </c>
+      <c r="I12" s="72">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="J12" s="72">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="M12" s="15"/>
-      <c r="N12" s="18"/>
+      <c r="N12" s="18">
+        <v>41845</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="50" t="s">
+        <v>120</v>
+      </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
-      <c r="J13" s="4"/>
+      <c r="C13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2</v>
+      </c>
+      <c r="I13" s="72">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="J13" s="72">
+        <v>0.13194444444444445</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="M13" s="15"/>
-      <c r="N13" s="18"/>
+      <c r="N13" s="18">
+        <v>41845</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
+      <c r="A14" s="73" t="s">
+        <v>121</v>
+      </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
+      <c r="C14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="4">
+        <v>4</v>
+      </c>
       <c r="J14" s="4"/>
       <c r="K14" s="2"/>
       <c r="M14" s="15"/>
-      <c r="N14" s="18"/>
+      <c r="N14" s="18">
+        <v>41850</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="55"/>
@@ -8159,18 +8325,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8288,6 +8454,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A72C14-AAB0-41A8-AF9B-22D04EB8DF14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF3CF34B-E2F6-4638-94A3-0D272C4219B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -8298,14 +8472,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A72C14-AAB0-41A8-AF9B-22D04EB8DF14}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@10/10/2014 12:36:14 PM] updated through 10/10
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13730
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
+++ b/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="600" windowWidth="18900" windowHeight="4872" activeTab="3"/>
+    <workbookView xWindow="-5160" yWindow="516" windowWidth="18900" windowHeight="4872" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Velocity Size Defs" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="145">
   <si>
     <t xml:space="preserve">Priority   </t>
   </si>
@@ -413,7 +413,67 @@
     <t>Quality and Supervisor eCL</t>
   </si>
   <si>
-    <t>Active</t>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Review V&amp;V</t>
+  </si>
+  <si>
+    <t>13466 - Manual eCL inactivations for September</t>
+  </si>
+  <si>
+    <t>Pending Info</t>
+  </si>
+  <si>
+    <t>13467 - User Checks on servers</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Split Dev &amp; V&amp;V</t>
+  </si>
+  <si>
+    <t>13506 - ARC CSRs to submit eCLs</t>
+  </si>
+  <si>
+    <t>13512 - Display employee instead of CSR on all review pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jourdain </t>
+  </si>
+  <si>
+    <t>13515 - update email notification mappings for sup and quality modules</t>
+  </si>
+  <si>
+    <t>13531 - update URL in notification script</t>
+  </si>
+  <si>
+    <t>13542 - Add warning question to eCL Supervisor</t>
+  </si>
+  <si>
+    <t>13479 - Add CSR warning to eCL</t>
+  </si>
+  <si>
+    <t>13549 - update eCL to remove PII</t>
+  </si>
+  <si>
+    <t>Doug, Jourdain, Suzy</t>
+  </si>
+  <si>
+    <t>13571 - Fix incorrect submitterID values on eCLs</t>
+  </si>
+  <si>
+    <t>13609 - Add quality alignment specialists to receive eCLs</t>
+  </si>
+  <si>
+    <t>Jourdain, Suzy, Doug</t>
   </si>
 </sst>
 </file>
@@ -670,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -852,6 +912,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5601,7 +5662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F44" sqref="F44"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
@@ -5811,7 +5872,7 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="50" t="s">
@@ -5853,7 +5914,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>56</v>
@@ -5867,14 +5928,17 @@
       <c r="I9" s="71">
         <v>1.3333333333333333</v>
       </c>
-      <c r="J9" s="4">
-        <v>0</v>
+      <c r="J9" s="72">
+        <v>0.88541666666666663</v>
       </c>
       <c r="K9" s="2"/>
       <c r="M9" s="15"/>
       <c r="N9" s="18">
         <v>41800</v>
       </c>
+      <c r="O9" s="17">
+        <v>41865</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="73" t="s">
@@ -5888,7 +5952,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>56</v>
@@ -5903,7 +5967,7 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="J10" s="72">
-        <v>0.1423611111111111</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="K10" s="2"/>
       <c r="M10" s="15"/>
@@ -6808,10 +6872,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6819,8 +6883,10 @@
     <col min="1" max="1" width="53.5546875" customWidth="1"/>
     <col min="2" max="2" width="9.109375" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6901,7 +6967,9 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="F3" t="s">
         <v>58</v>
       </c>
@@ -6932,7 +7000,9 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="F4" t="s">
         <v>58</v>
       </c>
@@ -6964,7 +7034,9 @@
       <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="F5" t="s">
         <v>58</v>
       </c>
@@ -7052,58 +7124,325 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
     </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="62">
+        <v>0.53125</v>
+      </c>
+      <c r="N13" s="60">
+        <v>41884</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="N14" s="60">
+        <v>41884</v>
+      </c>
+    </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15" s="75">
+        <v>4.229166666666667</v>
+      </c>
+      <c r="J15" s="62">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="N15" s="60">
+        <v>41892</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="62">
+        <v>0.25</v>
+      </c>
+      <c r="J16" s="62">
+        <v>0.21875</v>
+      </c>
+      <c r="N16" s="60">
+        <v>41894</v>
+      </c>
+      <c r="O16" s="60">
+        <v>41904</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A17" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="75">
+        <v>1.0069444444444444</v>
+      </c>
+      <c r="J17" s="62">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="N17" s="60">
+        <v>41897</v>
+      </c>
+      <c r="O17" s="60">
+        <v>41907</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="75">
+        <v>1.1736111111111112</v>
+      </c>
+      <c r="J18" s="62">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="N18" s="60">
+        <v>41897</v>
+      </c>
+      <c r="O18" s="60">
+        <v>41918</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-    </row>
-    <row r="21" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A19" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="62">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="J19" s="62">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="N19" s="60">
+        <v>41901</v>
+      </c>
+      <c r="O19" s="60">
+        <v>41907</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" t="s">
+        <v>141</v>
+      </c>
+      <c r="N20" s="60">
+        <v>41907</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="62">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="N21" s="60">
+        <v>41911</v>
+      </c>
+      <c r="O21" s="60">
+        <v>41911</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
-    </row>
-    <row r="26" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="43"/>
+    </row>
+    <row r="28" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7114,8 +7453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7124,6 +7463,7 @@
     <col min="2" max="2" width="9.109375" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7383,11 +7723,59 @@
       <c r="O11" s="43"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="G13" s="7"/>
+      <c r="A12" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="62">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="N12" s="60">
+        <v>41915</v>
+      </c>
+      <c r="O12" s="60">
+        <v>41918</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="N13" s="60">
+        <v>41920</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="59"/>
@@ -8325,18 +8713,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8454,24 +8842,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A72C14-AAB0-41A8-AF9B-22D04EB8DF14}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF3CF34B-E2F6-4638-94A3-0D272C4219B5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF3CF34B-E2F6-4638-94A3-0D272C4219B5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A72C14-AAB0-41A8-AF9B-22D04EB8DF14}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@10/15/2014 12:56:14 PM] updated 10/15/2014
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13741
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
+++ b/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="152">
   <si>
     <t xml:space="preserve">Priority   </t>
   </si>
@@ -419,9 +419,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Review V&amp;V</t>
-  </si>
-  <si>
     <t>13466 - Manual eCL inactivations for September</t>
   </si>
   <si>
@@ -474,6 +471,30 @@
   </si>
   <si>
     <t>Jourdain, Suzy, Doug</t>
+  </si>
+  <si>
+    <t>34:50</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>13618 - CCO eCoaching - Update dashboards to add check for current lanid association</t>
+  </si>
+  <si>
+    <t>13622 - eCoaching - Review Page OMR Research SOP Link</t>
+  </si>
+  <si>
+    <t>Review IA</t>
+  </si>
+  <si>
+    <t>13623 - CCO eCoaching - Load process for historical warning logs</t>
+  </si>
+  <si>
+    <t>13624 - eCoaching - Warnings to be inactivated after 13 weeks</t>
+  </si>
+  <si>
+    <t>13621 - eCoaching - Coaching Notes overwritten</t>
   </si>
 </sst>
 </file>
@@ -730,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -913,6 +934,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5665,7 +5689,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F44" sqref="F44"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5952,7 +5976,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>56</v>
@@ -5974,6 +5998,9 @@
       <c r="N10" s="18">
         <v>41802</v>
       </c>
+      <c r="O10" s="17">
+        <v>41926</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="73" t="s">
@@ -5987,7 +6014,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>56</v>
@@ -6001,12 +6028,17 @@
       <c r="I11" s="71">
         <v>1.2569444444444444</v>
       </c>
-      <c r="J11" s="72"/>
+      <c r="J11" s="76" t="s">
+        <v>144</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="M11" s="15"/>
       <c r="N11" s="18">
         <v>41814</v>
       </c>
+      <c r="O11" s="17">
+        <v>41865</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="73" t="s">
@@ -6020,7 +6052,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>56</v>
@@ -6035,13 +6067,16 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="J12" s="72">
-        <v>1.3888888888888888E-2</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="K12" s="2"/>
       <c r="M12" s="15"/>
       <c r="N12" s="18">
         <v>41845</v>
       </c>
+      <c r="O12" s="17">
+        <v>41865</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="50" t="s">
@@ -6055,7 +6090,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>56</v>
@@ -6070,13 +6105,16 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="J13" s="72">
-        <v>0.13194444444444445</v>
+        <v>0.2951388888888889</v>
       </c>
       <c r="K13" s="2"/>
       <c r="M13" s="15"/>
       <c r="N13" s="18">
         <v>41845</v>
       </c>
+      <c r="O13" s="17">
+        <v>41865</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="73" t="s">
@@ -6090,7 +6128,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>58</v>
@@ -6875,7 +6913,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7126,7 +7164,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -7135,7 +7173,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F13" t="s">
         <v>58</v>
@@ -7155,7 +7193,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -7164,13 +7202,13 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F14" t="s">
         <v>59</v>
       </c>
       <c r="G14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -7181,7 +7219,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -7190,7 +7228,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F15" t="s">
         <v>59</v>
@@ -7213,7 +7251,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -7248,7 +7286,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -7263,7 +7301,7 @@
         <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -7283,7 +7321,7 @@
     </row>
     <row r="18" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -7318,7 +7356,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19">
         <v>6</v>
@@ -7353,19 +7391,19 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
         <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N20" s="60">
         <v>41907</v>
@@ -7373,7 +7411,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B21">
         <v>7</v>
@@ -7451,10 +7489,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7463,7 +7501,7 @@
     <col min="2" max="2" width="9.109375" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7724,7 +7762,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -7759,69 +7797,171 @@
     </row>
     <row r="13" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F13" t="s">
         <v>60</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N13" s="60">
         <v>41920</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+    <row r="14" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N14" s="60">
+        <v>41925</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H15" s="62">
+        <v>0.25694444444444448</v>
+      </c>
+      <c r="N15" s="60">
+        <v>41926</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N16" s="60">
+        <v>41926</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N17" s="60">
+        <v>41926</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N18" s="60">
+        <v>41926</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="59"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="7"/>
+      <c r="N19" s="60"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="43"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="43"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8713,18 +8853,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8842,6 +8982,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A72C14-AAB0-41A8-AF9B-22D04EB8DF14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF3CF34B-E2F6-4638-94A3-0D272C4219B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -8852,14 +9000,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A72C14-AAB0-41A8-AF9B-22D04EB8DF14}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@11/14/2014 3:08:16 PM] updated for Oct and Nov
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13801
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
+++ b/Project Management/CCO OY2_eCoahing Log Work Items List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-5160" yWindow="516" windowWidth="18900" windowHeight="4872" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="18900" windowHeight="9540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Velocity Size Defs" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="170">
   <si>
     <t xml:space="preserve">Priority   </t>
   </si>
@@ -428,9 +428,6 @@
     <t>13467 - User Checks on servers</t>
   </si>
   <si>
-    <t>IA</t>
-  </si>
-  <si>
     <t>Tim</t>
   </si>
   <si>
@@ -485,16 +482,73 @@
     <t>13622 - eCoaching - Review Page OMR Research SOP Link</t>
   </si>
   <si>
-    <t>Review IA</t>
-  </si>
-  <si>
     <t>13623 - CCO eCoaching - Load process for historical warning logs</t>
   </si>
   <si>
     <t>13624 - eCoaching - Warnings to be inactivated after 13 weeks</t>
   </si>
   <si>
-    <t>13621 - eCoaching - Coaching Notes overwritten</t>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>V&amp;V</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>13631 - eCoaching - Coaching Notes overwritten</t>
+  </si>
+  <si>
+    <t>13653 - eCoaching - LSA Module</t>
+  </si>
+  <si>
+    <t>13659 - eCoaching - ETS data feed</t>
+  </si>
+  <si>
+    <t>13694 - CCO eCoaching - Fix incorrect submitterid value for IQS logs</t>
+  </si>
+  <si>
+    <t>13753 - eCoaching - grant rights to the Operations SR. Exec Mgmt</t>
+  </si>
+  <si>
+    <t>13759 - eCoaching Log - mask/handle names with apostrophe in dashboard sorting queries.</t>
+  </si>
+  <si>
+    <t>Size estimate (Hours)</t>
+  </si>
+  <si>
+    <t>IA review</t>
+  </si>
+  <si>
+    <t>Suzy, doug</t>
+  </si>
+  <si>
+    <t>13794 - eCoaching Log - Update supervisor pending to allow for acting manager view</t>
+  </si>
+  <si>
+    <t>13822 - eCoaching - Disable review for ARCs on My Submissions page</t>
+  </si>
+  <si>
+    <t>13833 - eCoaching - Changing employee causes different results with Warnings</t>
+  </si>
+  <si>
+    <t>Size estimate (Hourss)</t>
+  </si>
+  <si>
+    <t>Doug, Suzy</t>
+  </si>
+  <si>
+    <t>Suzy, Doug, Jourdain</t>
+  </si>
+  <si>
+    <t>Jourdain, Doug</t>
   </si>
 </sst>
 </file>
@@ -1244,21 +1298,21 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -1269,7 +1323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10">
         <v>1</v>
       </c>
@@ -1280,7 +1334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
         <v>2</v>
       </c>
@@ -1291,7 +1345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
         <v>3</v>
       </c>
@@ -1302,7 +1356,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>4</v>
       </c>
@@ -1313,7 +1367,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>5</v>
       </c>
@@ -1324,7 +1378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="22">
         <v>6</v>
       </c>
@@ -1335,7 +1389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="22">
         <v>7</v>
@@ -1347,7 +1401,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="22">
         <v>8</v>
       </c>
@@ -1358,7 +1412,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22">
         <v>9</v>
       </c>
@@ -1369,7 +1423,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22">
         <v>10</v>
       </c>
@@ -1380,7 +1434,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="22">
         <v>11</v>
       </c>
@@ -1391,7 +1445,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22">
         <v>12</v>
       </c>
@@ -1402,7 +1456,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22">
         <v>13</v>
       </c>
@@ -1427,20 +1481,20 @@
       <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -1487,7 +1541,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -1506,7 +1560,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -1530,7 +1584,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1556,7 +1610,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -1582,7 +1636,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
@@ -1599,7 +1653,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -1616,7 +1670,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
@@ -1633,7 +1687,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
@@ -1652,41 +1706,41 @@
       <c r="N9" s="42"/>
       <c r="O9" s="43"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="59"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="59"/>
       <c r="N12" s="60"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="59"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="59"/>
       <c r="N15" s="60"/>
       <c r="O15" s="60"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="59"/>
       <c r="N16" s="60"/>
       <c r="O16" s="60"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="44" t="s">
         <v>23</v>
       </c>
@@ -1705,7 +1759,7 @@
       <c r="N18" s="42"/>
       <c r="O18" s="43"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
         <v>8</v>
       </c>
@@ -1737,19 +1791,19 @@
       <selection activeCell="A6" sqref="A6:O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -1796,7 +1850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -1815,7 +1869,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -1839,7 +1893,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1865,7 +1919,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -1891,7 +1945,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="19"/>
       <c r="C6" s="6"/>
@@ -1906,7 +1960,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
@@ -1921,7 +1975,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="19"/>
       <c r="C8" s="6"/>
@@ -1936,7 +1990,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
@@ -1955,41 +2009,41 @@
       <c r="N9" s="42"/>
       <c r="O9" s="43"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="E10" s="2"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="59"/>
       <c r="E11" s="2"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="59"/>
       <c r="E12" s="2"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
       <c r="E13" s="2"/>
       <c r="N13" s="60"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="59"/>
       <c r="E14" s="2"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="59"/>
       <c r="E15" s="2"/>
       <c r="N15" s="60"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="59"/>
       <c r="E16" s="2"/>
       <c r="I16" s="62"/>
@@ -1997,7 +2051,7 @@
       <c r="N16" s="60"/>
       <c r="O16" s="60"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="44" t="s">
         <v>23</v>
       </c>
@@ -2016,7 +2070,7 @@
       <c r="N18" s="42"/>
       <c r="O18" s="43"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
         <v>8</v>
       </c>
@@ -2048,18 +2102,18 @@
       <selection activeCell="A6" sqref="A6:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -2106,7 +2160,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -2125,7 +2179,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -2149,7 +2203,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -2175,7 +2229,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -2201,7 +2255,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="19"/>
       <c r="C6" s="6"/>
@@ -2216,7 +2270,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
@@ -2231,7 +2285,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="19"/>
       <c r="C8" s="6"/>
@@ -2246,7 +2300,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
@@ -2265,39 +2319,39 @@
       <c r="N9" s="42"/>
       <c r="O9" s="43"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="F10" s="1"/>
       <c r="N10" s="60"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="59"/>
       <c r="C11" s="6"/>
       <c r="F11" s="1"/>
       <c r="N11" s="60"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="59"/>
       <c r="C12" s="6"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="N12" s="60"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="59"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="59"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="59"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="44" t="s">
         <v>23</v>
       </c>
@@ -2316,7 +2370,7 @@
       <c r="N18" s="42"/>
       <c r="O18" s="43"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
         <v>8</v>
       </c>
@@ -2348,18 +2402,18 @@
       <selection activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -2406,7 +2460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -2425,7 +2479,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -2449,7 +2503,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -2475,7 +2529,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -2501,7 +2555,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="19"/>
       <c r="C6" s="6"/>
@@ -2516,7 +2570,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
@@ -2531,7 +2585,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="19"/>
       <c r="C8" s="6"/>
@@ -2546,7 +2600,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
@@ -2565,15 +2619,15 @@
       <c r="N9" s="42"/>
       <c r="O9" s="43"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="59"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="44" t="s">
         <v>23</v>
       </c>
@@ -2592,7 +2646,7 @@
       <c r="N18" s="42"/>
       <c r="O18" s="43"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
         <v>8</v>
       </c>
@@ -2626,25 +2680,25 @@
       <selection pane="bottomLeft" activeCell="A24" sqref="A24:O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="9" width="10.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -2691,7 +2745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -2710,7 +2764,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -2741,7 +2795,7 @@
       </c>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -2773,7 +2827,7 @@
       <c r="K4" s="1"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -2805,7 +2859,7 @@
       <c r="K5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="19"/>
       <c r="C6" s="6"/>
@@ -2818,7 +2872,7 @@
       <c r="K6" s="1"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
@@ -2831,7 +2885,7 @@
       <c r="K7" s="1"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>24</v>
       </c>
@@ -2850,7 +2904,7 @@
       <c r="N8" s="42"/>
       <c r="O8" s="43"/>
     </row>
-    <row r="9" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="73" t="s">
         <v>78</v>
       </c>
@@ -2885,7 +2939,7 @@
         <v>41800</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="73" t="s">
         <v>80</v>
       </c>
@@ -2920,7 +2974,7 @@
         <v>41802</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="73" t="s">
         <v>84</v>
       </c>
@@ -2958,7 +3012,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="73" t="s">
         <v>88</v>
       </c>
@@ -2996,7 +3050,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="73" t="s">
         <v>90</v>
       </c>
@@ -3034,7 +3088,7 @@
         <v>41809</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="73" t="s">
         <v>91</v>
       </c>
@@ -3072,7 +3126,7 @@
         <v>41830</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
         <v>94</v>
       </c>
@@ -3110,7 +3164,7 @@
         <v>41816</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="73" t="s">
         <v>95</v>
       </c>
@@ -3148,7 +3202,7 @@
         <v>41830</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="73" t="s">
         <v>97</v>
       </c>
@@ -3186,7 +3240,7 @@
         <v>41813</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="74" t="s">
         <v>98</v>
       </c>
@@ -3221,7 +3275,7 @@
         <v>41808</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="74" t="s">
         <v>99</v>
       </c>
@@ -3259,7 +3313,7 @@
         <v>41813</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="73" t="s">
         <v>100</v>
       </c>
@@ -3297,7 +3351,7 @@
         <v>41827</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="73" t="s">
         <v>101</v>
       </c>
@@ -3335,7 +3389,7 @@
         <v>41830</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="73" t="s">
         <v>102</v>
       </c>
@@ -3373,7 +3427,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="73" t="s">
         <v>103</v>
       </c>
@@ -3411,7 +3465,7 @@
         <v>41834</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="73" t="s">
         <v>104</v>
       </c>
@@ -3444,7 +3498,7 @@
         <v>41814</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="73"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -3457,7 +3511,7 @@
       <c r="M25" s="15"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="1:15" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
         <v>51</v>
       </c>
@@ -3499,7 +3553,7 @@
       </c>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="70" t="s">
         <v>69</v>
       </c>
@@ -3518,7 +3572,7 @@
       <c r="N27" s="69"/>
       <c r="O27" s="69"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="50" t="s">
         <v>70</v>
       </c>
@@ -3542,7 +3596,7 @@
       <c r="M28" s="15"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="50" t="s">
         <v>71</v>
       </c>
@@ -3566,7 +3620,7 @@
       <c r="M29" s="15"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="50" t="s">
         <v>75</v>
       </c>
@@ -3588,7 +3642,7 @@
       <c r="M30" s="15"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="55"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
@@ -3600,7 +3654,7 @@
       <c r="M31" s="15"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="55"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
@@ -3612,7 +3666,7 @@
       <c r="M32" s="15"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="56"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -3624,7 +3678,7 @@
       <c r="M33" s="15"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="55"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
@@ -3636,7 +3690,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="55"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -3648,7 +3702,7 @@
       <c r="M35" s="15"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
@@ -3660,7 +3714,7 @@
       <c r="M36" s="15"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
@@ -3672,7 +3726,7 @@
       <c r="M37" s="15"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="54"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
@@ -3684,7 +3738,7 @@
       <c r="M38" s="15"/>
       <c r="N38" s="18"/>
     </row>
-    <row r="39" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
@@ -3696,7 +3750,7 @@
       <c r="M39" s="15"/>
       <c r="N39" s="18"/>
     </row>
-    <row r="40" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
@@ -3708,7 +3762,7 @@
       <c r="M40" s="15"/>
       <c r="N40" s="18"/>
     </row>
-    <row r="41" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
@@ -3720,7 +3774,7 @@
       <c r="M41" s="15"/>
       <c r="N41" s="18"/>
     </row>
-    <row r="42" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
@@ -3732,7 +3786,7 @@
       <c r="M42" s="15"/>
       <c r="N42" s="18"/>
     </row>
-    <row r="43" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
@@ -3744,7 +3798,7 @@
       <c r="M43" s="15"/>
       <c r="N43" s="18"/>
     </row>
-    <row r="44" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="54"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
@@ -3756,7 +3810,7 @@
       <c r="M44" s="15"/>
       <c r="N44" s="18"/>
     </row>
-    <row r="45" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="55"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
@@ -3768,7 +3822,7 @@
       <c r="M45" s="15"/>
       <c r="N45" s="18"/>
     </row>
-    <row r="46" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="55"/>
       <c r="B46" s="5"/>
       <c r="C46" s="6"/>
@@ -3780,7 +3834,7 @@
       <c r="M46" s="15"/>
       <c r="N46" s="18"/>
     </row>
-    <row r="47" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="55"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
@@ -3792,7 +3846,7 @@
       <c r="M47" s="15"/>
       <c r="N47" s="18"/>
     </row>
-    <row r="48" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="55"/>
       <c r="B48" s="5"/>
       <c r="C48" s="6"/>
@@ -3804,7 +3858,7 @@
       <c r="M48" s="15"/>
       <c r="N48" s="18"/>
     </row>
-    <row r="49" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -3816,7 +3870,7 @@
       <c r="M49" s="15"/>
       <c r="N49" s="18"/>
     </row>
-    <row r="50" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="54"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
@@ -3828,7 +3882,7 @@
       <c r="M50" s="15"/>
       <c r="N50" s="18"/>
     </row>
-    <row r="51" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="55"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
@@ -3840,7 +3894,7 @@
       <c r="M51" s="15"/>
       <c r="N51" s="18"/>
     </row>
-    <row r="52" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
@@ -3852,7 +3906,7 @@
       <c r="M52" s="15"/>
       <c r="N52" s="18"/>
     </row>
-    <row r="53" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="54"/>
       <c r="B53" s="5"/>
       <c r="C53" s="6"/>
@@ -3864,7 +3918,7 @@
       <c r="M53" s="15"/>
       <c r="N53" s="18"/>
     </row>
-    <row r="54" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="55"/>
       <c r="B54" s="5"/>
       <c r="C54" s="6"/>
@@ -3876,7 +3930,7 @@
       <c r="M54" s="15"/>
       <c r="N54" s="18"/>
     </row>
-    <row r="55" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="55"/>
       <c r="B55" s="5"/>
       <c r="C55" s="6"/>
@@ -3888,7 +3942,7 @@
       <c r="M55" s="15"/>
       <c r="N55" s="18"/>
     </row>
-    <row r="56" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="55"/>
       <c r="B56" s="5"/>
       <c r="C56" s="6"/>
@@ -3900,7 +3954,7 @@
       <c r="M56" s="15"/>
       <c r="N56" s="18"/>
     </row>
-    <row r="57" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="5"/>
       <c r="C57" s="6"/>
@@ -3912,7 +3966,7 @@
       <c r="M57" s="15"/>
       <c r="N57" s="18"/>
     </row>
-    <row r="58" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="5"/>
       <c r="C58" s="6"/>
@@ -3924,7 +3978,7 @@
       <c r="M58" s="15"/>
       <c r="N58" s="18"/>
     </row>
-    <row r="59" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="5"/>
       <c r="C59" s="6"/>
@@ -3936,7 +3990,7 @@
       <c r="M59" s="15"/>
       <c r="N59" s="18"/>
     </row>
-    <row r="60" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="5"/>
       <c r="C60" s="6"/>
@@ -3948,7 +4002,7 @@
       <c r="M60" s="15"/>
       <c r="N60" s="18"/>
     </row>
-    <row r="61" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="5"/>
       <c r="C61" s="6"/>
@@ -3960,7 +4014,7 @@
       <c r="M61" s="15"/>
       <c r="N61" s="18"/>
     </row>
-    <row r="62" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="5"/>
       <c r="C62" s="6"/>
@@ -3972,7 +4026,7 @@
       <c r="M62" s="15"/>
       <c r="N62" s="18"/>
     </row>
-    <row r="63" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="5"/>
       <c r="C63" s="6"/>
@@ -3984,7 +4038,7 @@
       <c r="M63" s="15"/>
       <c r="N63" s="18"/>
     </row>
-    <row r="64" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="5"/>
       <c r="C64" s="6"/>
@@ -3996,7 +4050,7 @@
       <c r="M64" s="15"/>
       <c r="N64" s="18"/>
     </row>
-    <row r="65" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="5"/>
       <c r="C65" s="6"/>
@@ -4009,7 +4063,7 @@
       <c r="L65" s="16"/>
       <c r="M65" s="2"/>
     </row>
-    <row r="66" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="44" t="s">
         <v>23</v>
       </c>
@@ -4028,7 +4082,7 @@
       <c r="N66" s="42"/>
       <c r="O66" s="43"/>
     </row>
-    <row r="67" spans="1:15" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="5"/>
       <c r="C67" s="6"/>
@@ -4045,7 +4099,7 @@
       <c r="N67" s="18"/>
       <c r="O67" s="18"/>
     </row>
-    <row r="68" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="5"/>
       <c r="E68" s="1"/>
@@ -4058,7 +4112,7 @@
       <c r="L68" s="16"/>
       <c r="M68" s="2"/>
     </row>
-    <row r="69" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="5"/>
       <c r="C69" s="6"/>
@@ -4068,7 +4122,7 @@
       <c r="K69" s="1"/>
       <c r="M69" s="2"/>
     </row>
-    <row r="70" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="5"/>
       <c r="C70" s="6"/>
@@ -4078,7 +4132,7 @@
       <c r="K70" s="1"/>
       <c r="M70" s="2"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="5"/>
       <c r="C71" s="6"/>
@@ -4088,7 +4142,7 @@
       <c r="G71" s="1"/>
       <c r="M71" s="2"/>
     </row>
-    <row r="72" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="45" t="s">
         <v>8</v>
       </c>
@@ -4107,7 +4161,7 @@
       <c r="N72" s="49"/>
       <c r="O72" s="49"/>
     </row>
-    <row r="73" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -4118,7 +4172,7 @@
       <c r="H73" s="6"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -4129,7 +4183,7 @@
       <c r="H74" s="6"/>
       <c r="M74" s="2"/>
     </row>
-    <row r="75" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -4141,7 +4195,7 @@
       <c r="J75" s="4"/>
       <c r="M75" s="2"/>
     </row>
-    <row r="76" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -4151,7 +4205,7 @@
       <c r="G76" s="2"/>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" spans="1:15" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -4161,7 +4215,7 @@
       <c r="G77" s="2"/>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -4172,7 +4226,7 @@
       <c r="H78" s="6"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -4183,7 +4237,7 @@
       <c r="H79" s="6"/>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="5"/>
       <c r="D80" s="6"/>
@@ -4191,7 +4245,7 @@
       <c r="G80" s="2"/>
       <c r="M80" s="2"/>
     </row>
-    <row r="81" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="5"/>
       <c r="C81" s="6"/>
@@ -4199,7 +4253,7 @@
       <c r="G81" s="2"/>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="5"/>
       <c r="C82" s="6"/>
@@ -4209,19 +4263,19 @@
       <c r="G82" s="2"/>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" spans="1:13" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="5"/>
       <c r="F83" s="1"/>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="1:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="5"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="5"/>
       <c r="C86" s="6"/>
@@ -4229,23 +4283,23 @@
       <c r="F86" s="1"/>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="5"/>
       <c r="C88" s="6"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="C89" s="6"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
@@ -4254,26 +4308,26 @@
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="C91" s="6"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="6"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="C92" s="6"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="C93" s="6"/>
       <c r="F93" s="1"/>
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94"/>
       <c r="B94" s="4"/>
       <c r="E94" s="4"/>
@@ -4294,25 +4348,25 @@
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="9" width="10.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -4359,7 +4413,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -4378,7 +4432,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -4407,7 +4461,7 @@
       </c>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -4437,7 +4491,7 @@
       <c r="K4" s="1"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -4467,7 +4521,7 @@
       <c r="K5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="19"/>
       <c r="C6" s="6"/>
@@ -4480,7 +4534,7 @@
       <c r="K6" s="1"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
@@ -4493,7 +4547,7 @@
       <c r="K7" s="1"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>24</v>
       </c>
@@ -4512,7 +4566,7 @@
       <c r="N8" s="42"/>
       <c r="O8" s="43"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="73" t="s">
         <v>105</v>
       </c>
@@ -4545,7 +4599,7 @@
         <v>41821</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="73" t="s">
         <v>107</v>
       </c>
@@ -4583,7 +4637,7 @@
         <v>41830</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="73" t="s">
         <v>108</v>
       </c>
@@ -4621,7 +4675,7 @@
         <v>41841</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="73" t="s">
         <v>110</v>
       </c>
@@ -4659,7 +4713,7 @@
         <v>41841</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="73" t="s">
         <v>112</v>
       </c>
@@ -4692,7 +4746,7 @@
         <v>41830</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="73" t="s">
         <v>114</v>
       </c>
@@ -4722,7 +4776,7 @@
         <v>41830</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
         <v>115</v>
       </c>
@@ -4752,7 +4806,7 @@
         <v>41837</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="73" t="s">
         <v>116</v>
       </c>
@@ -4782,7 +4836,7 @@
         <v>41838</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="55"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -4794,7 +4848,7 @@
       <c r="M17" s="15"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="56"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -4806,7 +4860,7 @@
       <c r="M18" s="15"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="55"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -4818,7 +4872,7 @@
       <c r="M19" s="15"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="55"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -4830,7 +4884,7 @@
       <c r="M20" s="15"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
@@ -4842,7 +4896,7 @@
       <c r="M21" s="15"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="55"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
@@ -4854,7 +4908,7 @@
       <c r="M22" s="15"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="56"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
@@ -4866,7 +4920,7 @@
       <c r="M23" s="15"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
@@ -4878,7 +4932,7 @@
       <c r="M24" s="15"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="55"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
@@ -4890,7 +4944,7 @@
       <c r="M25" s="15"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="55"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
@@ -4902,7 +4956,7 @@
       <c r="M26" s="15"/>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="55"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
@@ -4914,7 +4968,7 @@
       <c r="M27" s="15"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="56"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
@@ -4926,7 +4980,7 @@
       <c r="M28" s="15"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="55"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
@@ -4938,7 +4992,7 @@
       <c r="M29" s="15"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="55"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
@@ -4950,7 +5004,7 @@
       <c r="M30" s="15"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="54"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
@@ -4962,7 +5016,7 @@
       <c r="M31" s="15"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="55"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
@@ -4974,7 +5028,7 @@
       <c r="M32" s="15"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="55"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -4986,7 +5040,7 @@
       <c r="M33" s="15"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="55"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
@@ -4998,7 +5052,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="55"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -5010,7 +5064,7 @@
       <c r="M35" s="15"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
@@ -5022,7 +5076,7 @@
       <c r="M36" s="15"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="56"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
@@ -5034,7 +5088,7 @@
       <c r="M37" s="15"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="55"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
@@ -5046,7 +5100,7 @@
       <c r="M38" s="15"/>
       <c r="N38" s="18"/>
     </row>
-    <row r="39" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="55"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
@@ -5058,7 +5112,7 @@
       <c r="M39" s="15"/>
       <c r="N39" s="18"/>
     </row>
-    <row r="40" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="55"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
@@ -5070,7 +5124,7 @@
       <c r="M40" s="15"/>
       <c r="N40" s="18"/>
     </row>
-    <row r="41" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="55"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
@@ -5082,7 +5136,7 @@
       <c r="M41" s="15"/>
       <c r="N41" s="18"/>
     </row>
-    <row r="42" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="54"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
@@ -5094,7 +5148,7 @@
       <c r="M42" s="15"/>
       <c r="N42" s="18"/>
     </row>
-    <row r="43" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="55"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
@@ -5106,7 +5160,7 @@
       <c r="M43" s="15"/>
       <c r="N43" s="18"/>
     </row>
-    <row r="44" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="55"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
@@ -5118,7 +5172,7 @@
       <c r="M44" s="15"/>
       <c r="N44" s="18"/>
     </row>
-    <row r="45" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="55"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
@@ -5130,7 +5184,7 @@
       <c r="M45" s="15"/>
       <c r="N45" s="18"/>
     </row>
-    <row r="46" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="55"/>
       <c r="B46" s="5"/>
       <c r="C46" s="6"/>
@@ -5142,7 +5196,7 @@
       <c r="M46" s="15"/>
       <c r="N46" s="18"/>
     </row>
-    <row r="47" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="55"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
@@ -5154,7 +5208,7 @@
       <c r="M47" s="15"/>
       <c r="N47" s="18"/>
     </row>
-    <row r="48" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="54"/>
       <c r="B48" s="5"/>
       <c r="C48" s="6"/>
@@ -5166,7 +5220,7 @@
       <c r="M48" s="15"/>
       <c r="N48" s="18"/>
     </row>
-    <row r="49" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="55"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -5178,7 +5232,7 @@
       <c r="M49" s="15"/>
       <c r="N49" s="18"/>
     </row>
-    <row r="50" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="55"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
@@ -5190,7 +5244,7 @@
       <c r="M50" s="15"/>
       <c r="N50" s="18"/>
     </row>
-    <row r="51" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="55"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
@@ -5202,7 +5256,7 @@
       <c r="M51" s="15"/>
       <c r="N51" s="18"/>
     </row>
-    <row r="52" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="55"/>
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
@@ -5214,7 +5268,7 @@
       <c r="M52" s="15"/>
       <c r="N52" s="18"/>
     </row>
-    <row r="53" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="55"/>
       <c r="B53" s="5"/>
       <c r="C53" s="6"/>
@@ -5226,7 +5280,7 @@
       <c r="M53" s="15"/>
       <c r="N53" s="18"/>
     </row>
-    <row r="54" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="55"/>
       <c r="B54" s="5"/>
       <c r="C54" s="6"/>
@@ -5238,7 +5292,7 @@
       <c r="M54" s="15"/>
       <c r="N54" s="18"/>
     </row>
-    <row r="55" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="55"/>
       <c r="B55" s="5"/>
       <c r="C55" s="6"/>
@@ -5250,7 +5304,7 @@
       <c r="M55" s="15"/>
       <c r="N55" s="18"/>
     </row>
-    <row r="56" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="55"/>
       <c r="B56" s="5"/>
       <c r="C56" s="6"/>
@@ -5262,7 +5316,7 @@
       <c r="M56" s="15"/>
       <c r="N56" s="18"/>
     </row>
-    <row r="57" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="55"/>
       <c r="B57" s="5"/>
       <c r="C57" s="6"/>
@@ -5274,7 +5328,7 @@
       <c r="M57" s="15"/>
       <c r="N57" s="18"/>
     </row>
-    <row r="58" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="55"/>
       <c r="B58" s="5"/>
       <c r="C58" s="6"/>
@@ -5286,7 +5340,7 @@
       <c r="M58" s="15"/>
       <c r="N58" s="18"/>
     </row>
-    <row r="59" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="5"/>
       <c r="C59" s="6"/>
@@ -5299,7 +5353,7 @@
       <c r="L59" s="16"/>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="44" t="s">
         <v>23</v>
       </c>
@@ -5318,7 +5372,7 @@
       <c r="N60" s="42"/>
       <c r="O60" s="43"/>
     </row>
-    <row r="61" spans="1:15" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="5"/>
       <c r="C61" s="6"/>
@@ -5335,7 +5389,7 @@
       <c r="N61" s="18"/>
       <c r="O61" s="18"/>
     </row>
-    <row r="62" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="5"/>
       <c r="E62" s="1"/>
@@ -5348,7 +5402,7 @@
       <c r="L62" s="16"/>
       <c r="M62" s="2"/>
     </row>
-    <row r="63" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="5"/>
       <c r="C63" s="6"/>
@@ -5358,7 +5412,7 @@
       <c r="K63" s="1"/>
       <c r="M63" s="2"/>
     </row>
-    <row r="64" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="5"/>
       <c r="C64" s="6"/>
@@ -5368,7 +5422,7 @@
       <c r="K64" s="1"/>
       <c r="M64" s="2"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="5"/>
       <c r="C65" s="6"/>
@@ -5378,7 +5432,7 @@
       <c r="G65" s="1"/>
       <c r="M65" s="2"/>
     </row>
-    <row r="66" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="45" t="s">
         <v>8</v>
       </c>
@@ -5397,7 +5451,7 @@
       <c r="N66" s="49"/>
       <c r="O66" s="49"/>
     </row>
-    <row r="67" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -5408,7 +5462,7 @@
       <c r="H67" s="6"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -5419,7 +5473,7 @@
       <c r="H68" s="6"/>
       <c r="M68" s="2"/>
     </row>
-    <row r="69" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -5431,7 +5485,7 @@
       <c r="J69" s="4"/>
       <c r="M69" s="2"/>
     </row>
-    <row r="70" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -5441,7 +5495,7 @@
       <c r="G70" s="2"/>
       <c r="M70" s="2"/>
     </row>
-    <row r="71" spans="1:15" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -5451,7 +5505,7 @@
       <c r="G71" s="2"/>
       <c r="M71" s="2"/>
     </row>
-    <row r="72" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -5462,7 +5516,7 @@
       <c r="H72" s="6"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -5473,7 +5527,7 @@
       <c r="H73" s="6"/>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="5"/>
       <c r="D74" s="6"/>
@@ -5481,7 +5535,7 @@
       <c r="G74" s="2"/>
       <c r="M74" s="2"/>
     </row>
-    <row r="75" spans="1:15" s="17" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="17" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="5"/>
       <c r="C75" s="6"/>
@@ -5496,7 +5550,7 @@
       <c r="L75"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="1:15" s="17" customFormat="1" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" s="17" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="5"/>
       <c r="C76" s="6"/>
@@ -5511,7 +5565,7 @@
       <c r="L76"/>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" spans="1:15" s="17" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" s="17" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="5"/>
       <c r="C77" s="4"/>
@@ -5526,7 +5580,7 @@
       <c r="L77"/>
       <c r="M77"/>
     </row>
-    <row r="78" spans="1:15" s="17" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" s="17" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="5"/>
       <c r="C78" s="4"/>
@@ -5541,7 +5595,7 @@
       <c r="L78"/>
       <c r="M78"/>
     </row>
-    <row r="80" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="5"/>
       <c r="C80" s="6"/>
@@ -5556,7 +5610,7 @@
       <c r="L80"/>
       <c r="M80"/>
     </row>
-    <row r="81" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
       <c r="B81" s="20"/>
       <c r="C81" s="4"/>
@@ -5571,7 +5625,7 @@
       <c r="L81"/>
       <c r="M81"/>
     </row>
-    <row r="82" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="5"/>
       <c r="C82" s="6"/>
@@ -5586,7 +5640,7 @@
       <c r="L82"/>
       <c r="M82"/>
     </row>
-    <row r="83" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="20"/>
       <c r="C83" s="6"/>
@@ -5601,7 +5655,7 @@
       <c r="L83"/>
       <c r="M83"/>
     </row>
-    <row r="84" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="20"/>
       <c r="C84" s="6"/>
@@ -5616,7 +5670,7 @@
       <c r="L84"/>
       <c r="M84"/>
     </row>
-    <row r="85" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="20"/>
       <c r="C85" s="6"/>
@@ -5631,7 +5685,7 @@
       <c r="L85"/>
       <c r="M85"/>
     </row>
-    <row r="86" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="20"/>
       <c r="C86" s="6"/>
@@ -5646,7 +5700,7 @@
       <c r="L86"/>
       <c r="M86"/>
     </row>
-    <row r="87" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="20"/>
       <c r="C87" s="6"/>
@@ -5661,7 +5715,7 @@
       <c r="L87"/>
       <c r="M87"/>
     </row>
-    <row r="88" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -5687,30 +5741,30 @@
   <dimension ref="A1:O75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F44" sqref="F44"/>
       <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="9" width="10.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -5757,7 +5811,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -5776,7 +5830,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -5805,7 +5859,7 @@
       </c>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -5835,7 +5889,7 @@
       <c r="K4" s="1"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -5865,7 +5919,7 @@
       <c r="K5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>122</v>
       </c>
@@ -5884,7 +5938,7 @@
       <c r="N6" s="42"/>
       <c r="O6" s="43"/>
     </row>
-    <row r="7" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>123</v>
       </c>
@@ -5907,7 +5961,7 @@
       <c r="K7" s="1"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>118</v>
       </c>
@@ -5926,7 +5980,7 @@
       <c r="N8" s="42"/>
       <c r="O8" s="43"/>
     </row>
-    <row r="9" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="73" t="s">
         <v>78</v>
       </c>
@@ -5964,7 +6018,7 @@
         <v>41865</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="73" t="s">
         <v>80</v>
       </c>
@@ -6002,7 +6056,7 @@
         <v>41926</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="73" t="s">
         <v>104</v>
       </c>
@@ -6029,7 +6083,7 @@
         <v>1.2569444444444444</v>
       </c>
       <c r="J11" s="76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K11" s="2"/>
       <c r="M11" s="15"/>
@@ -6040,7 +6094,7 @@
         <v>41865</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="73" t="s">
         <v>119</v>
       </c>
@@ -6078,7 +6132,7 @@
         <v>41865</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="50" t="s">
         <v>120</v>
       </c>
@@ -6116,7 +6170,7 @@
         <v>41865</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="73" t="s">
         <v>121</v>
       </c>
@@ -6128,7 +6182,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>58</v>
@@ -6146,7 +6200,7 @@
         <v>41850</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="55"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -6158,7 +6212,7 @@
       <c r="M15" s="15"/>
       <c r="N15" s="18"/>
     </row>
-    <row r="16" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="55"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
@@ -6170,7 +6224,7 @@
       <c r="M16" s="15"/>
       <c r="N16" s="18"/>
     </row>
-    <row r="17" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="55"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -6182,7 +6236,7 @@
       <c r="M17" s="15"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="56"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -6194,7 +6248,7 @@
       <c r="M18" s="15"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="1:14" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="55"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -6206,7 +6260,7 @@
       <c r="M19" s="15"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -6218,7 +6272,7 @@
       <c r="M20" s="15"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
@@ -6230,7 +6284,7 @@
       <c r="M21" s="15"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="56"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
@@ -6242,7 +6296,7 @@
       <c r="M22" s="15"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="55"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
@@ -6254,7 +6308,7 @@
       <c r="M23" s="15"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
@@ -6266,7 +6320,7 @@
       <c r="M24" s="15"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="55"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
@@ -6278,7 +6332,7 @@
       <c r="M25" s="15"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="54"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
@@ -6290,7 +6344,7 @@
       <c r="M26" s="15"/>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="56"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
@@ -6302,7 +6356,7 @@
       <c r="M27" s="15"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="55"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
@@ -6314,7 +6368,7 @@
       <c r="M28" s="15"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="55"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
@@ -6326,7 +6380,7 @@
       <c r="M29" s="15"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="55"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
@@ -6338,7 +6392,7 @@
       <c r="M30" s="15"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="55"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
@@ -6350,7 +6404,7 @@
       <c r="M31" s="15"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="55"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
@@ -6362,7 +6416,7 @@
       <c r="M32" s="15"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="56"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -6374,7 +6428,7 @@
       <c r="M33" s="15"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="55"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
@@ -6386,7 +6440,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="55"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -6398,7 +6452,7 @@
       <c r="M35" s="15"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="55"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
@@ -6410,7 +6464,7 @@
       <c r="M36" s="15"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="55"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
@@ -6422,7 +6476,7 @@
       <c r="M37" s="15"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="54"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
@@ -6434,7 +6488,7 @@
       <c r="M38" s="15"/>
       <c r="N38" s="18"/>
     </row>
-    <row r="39" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="55"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
@@ -6446,7 +6500,7 @@
       <c r="M39" s="15"/>
       <c r="N39" s="18"/>
     </row>
-    <row r="40" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="55"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
@@ -6458,7 +6512,7 @@
       <c r="M40" s="15"/>
       <c r="N40" s="18"/>
     </row>
-    <row r="41" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="55"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
@@ -6470,13 +6524,13 @@
       <c r="M41" s="15"/>
       <c r="N41" s="18"/>
     </row>
-    <row r="42" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J42" s="4"/>
       <c r="K42" s="2"/>
       <c r="M42" s="15"/>
       <c r="N42" s="18"/>
     </row>
-    <row r="43" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="55"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
@@ -6488,7 +6542,7 @@
       <c r="M43" s="15"/>
       <c r="N43" s="18"/>
     </row>
-    <row r="44" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
@@ -6500,7 +6554,7 @@
       <c r="M44" s="15"/>
       <c r="N44" s="18"/>
     </row>
-    <row r="45" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
@@ -6512,7 +6566,7 @@
       <c r="M45" s="15"/>
       <c r="N45" s="18"/>
     </row>
-    <row r="46" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="5"/>
       <c r="C46" s="6"/>
@@ -6525,7 +6579,7 @@
       <c r="L46" s="16"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="44" t="s">
         <v>23</v>
       </c>
@@ -6544,7 +6598,7 @@
       <c r="N47" s="42"/>
       <c r="O47" s="43"/>
     </row>
-    <row r="48" spans="1:15" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="5"/>
       <c r="C48" s="6"/>
@@ -6561,7 +6615,7 @@
       <c r="N48" s="18"/>
       <c r="O48" s="18"/>
     </row>
-    <row r="49" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="5"/>
       <c r="E49" s="1"/>
@@ -6574,7 +6628,7 @@
       <c r="L49" s="16"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
@@ -6584,7 +6638,7 @@
       <c r="K50" s="1"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
@@ -6594,7 +6648,7 @@
       <c r="K51" s="1"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
@@ -6604,7 +6658,7 @@
       <c r="G52" s="1"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="45" t="s">
         <v>8</v>
       </c>
@@ -6623,7 +6677,7 @@
       <c r="N53" s="49"/>
       <c r="O53" s="49"/>
     </row>
-    <row r="54" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -6634,7 +6688,7 @@
       <c r="H54" s="6"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -6645,7 +6699,7 @@
       <c r="H55" s="6"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -6657,7 +6711,7 @@
       <c r="J56" s="4"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -6667,7 +6721,7 @@
       <c r="G57" s="2"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" spans="1:15" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -6677,7 +6731,7 @@
       <c r="G58" s="2"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -6688,7 +6742,7 @@
       <c r="H59" s="6"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -6699,7 +6753,7 @@
       <c r="H60" s="6"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="5"/>
       <c r="D61" s="6"/>
@@ -6707,7 +6761,7 @@
       <c r="G61" s="2"/>
       <c r="M61" s="2"/>
     </row>
-    <row r="62" spans="1:15" s="17" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="17" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="5"/>
       <c r="C62" s="6"/>
@@ -6722,7 +6776,7 @@
       <c r="L62"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="1:15" s="17" customFormat="1" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" s="17" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="5"/>
       <c r="C63" s="6"/>
@@ -6737,7 +6791,7 @@
       <c r="L63"/>
       <c r="M63" s="2"/>
     </row>
-    <row r="64" spans="1:15" s="17" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="17" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="5"/>
       <c r="C64" s="4"/>
@@ -6752,7 +6806,7 @@
       <c r="L64"/>
       <c r="M64"/>
     </row>
-    <row r="65" spans="1:13" s="17" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" s="17" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="5"/>
       <c r="C65" s="4"/>
@@ -6767,7 +6821,7 @@
       <c r="L65"/>
       <c r="M65"/>
     </row>
-    <row r="67" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="5"/>
       <c r="C67" s="6"/>
@@ -6782,7 +6836,7 @@
       <c r="L67"/>
       <c r="M67"/>
     </row>
-    <row r="68" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
       <c r="B68" s="20"/>
       <c r="C68" s="4"/>
@@ -6797,7 +6851,7 @@
       <c r="L68"/>
       <c r="M68"/>
     </row>
-    <row r="69" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="5"/>
       <c r="C69" s="6"/>
@@ -6812,7 +6866,7 @@
       <c r="L69"/>
       <c r="M69"/>
     </row>
-    <row r="70" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="20"/>
       <c r="C70" s="6"/>
@@ -6827,7 +6881,7 @@
       <c r="L70"/>
       <c r="M70"/>
     </row>
-    <row r="71" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="20"/>
       <c r="C71" s="6"/>
@@ -6842,7 +6896,7 @@
       <c r="L71"/>
       <c r="M71"/>
     </row>
-    <row r="72" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="20"/>
       <c r="C72" s="6"/>
@@ -6857,7 +6911,7 @@
       <c r="L72"/>
       <c r="M72"/>
     </row>
-    <row r="73" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="20"/>
       <c r="C73" s="6"/>
@@ -6872,7 +6926,7 @@
       <c r="L73"/>
       <c r="M73"/>
     </row>
-    <row r="74" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="20"/>
       <c r="C74" s="6"/>
@@ -6887,7 +6941,7 @@
       <c r="L74"/>
       <c r="M74"/>
     </row>
-    <row r="75" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -6912,23 +6966,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -6975,7 +7029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -6994,7 +7048,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -7027,7 +7081,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -7061,7 +7115,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -7095,13 +7149,13 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K6" s="1"/>
       <c r="M6" s="2"/>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="57"/>
       <c r="D7" s="6"/>
       <c r="K7" s="1"/>
@@ -7109,7 +7163,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="57"/>
       <c r="D8" s="6"/>
       <c r="K8" s="1"/>
@@ -7117,7 +7171,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="57"/>
       <c r="D9" s="6"/>
       <c r="K9" s="1"/>
@@ -7125,7 +7179,7 @@
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
     </row>
-    <row r="10" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="19"/>
       <c r="C10" s="6"/>
@@ -7140,7 +7194,7 @@
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
     </row>
-    <row r="11" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>24</v>
       </c>
@@ -7159,10 +7213,10 @@
       <c r="N11" s="42"/>
       <c r="O11" s="43"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -7191,7 +7245,7 @@
         <v>41884</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -7201,14 +7255,14 @@
       <c r="D14">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
-        <v>129</v>
+      <c r="E14" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="F14" t="s">
         <v>59</v>
       </c>
       <c r="G14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -7217,9 +7271,9 @@
         <v>41884</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -7228,7 +7282,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F15" t="s">
         <v>59</v>
@@ -7249,9 +7303,9 @@
         <v>41892</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -7284,9 +7338,9 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -7301,7 +7355,7 @@
         <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -7319,9 +7373,9 @@
         <v>41907</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -7354,9 +7408,9 @@
         <v>41918</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B19">
         <v>6</v>
@@ -7389,29 +7443,29 @@
         <v>41907</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20">
         <v>8</v>
       </c>
-      <c r="E20" t="s">
-        <v>129</v>
+      <c r="E20" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="F20" t="s">
         <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N20" s="60">
         <v>41907</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B21">
         <v>7</v>
@@ -7444,7 +7498,7 @@
         <v>41911</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="44" t="s">
         <v>23</v>
       </c>
@@ -7463,7 +7517,7 @@
       <c r="N23" s="42"/>
       <c r="O23" s="43"/>
     </row>
-    <row r="28" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45" t="s">
         <v>8</v>
       </c>
@@ -7489,23 +7543,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -7516,7 +7568,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>1</v>
@@ -7552,7 +7604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -7571,7 +7623,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -7602,7 +7654,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -7634,7 +7686,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -7666,7 +7718,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="19"/>
       <c r="C6" s="6"/>
@@ -7681,7 +7733,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
@@ -7696,7 +7748,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="19"/>
       <c r="C8" s="6"/>
@@ -7711,7 +7763,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="19"/>
       <c r="C9" s="6"/>
@@ -7726,7 +7778,7 @@
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="19"/>
       <c r="C10" s="6"/>
@@ -7741,7 +7793,7 @@
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>24</v>
       </c>
@@ -7760,17 +7812,17 @@
       <c r="N11" s="42"/>
       <c r="O11" s="43"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F12" t="s">
@@ -7795,173 +7847,321 @@
         <v>41918</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
-        <v>129</v>
+      <c r="D13" s="62">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F13" t="s">
         <v>60</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="J13" s="62">
+        <v>0.13541666666666666</v>
       </c>
       <c r="N13" s="60">
         <v>41920</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="O13" s="60">
+        <v>41953</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
+      <c r="D14" s="75">
+        <v>1.5069444444444444</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N14" s="60">
         <v>41925</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
+      <c r="D15" s="62">
+        <v>0.25694444444444448</v>
+      </c>
       <c r="E15" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="H15" s="62">
-        <v>0.25694444444444448</v>
+        <v>142</v>
+      </c>
+      <c r="H15" s="62"/>
+      <c r="J15" s="62">
+        <v>0.1763888888888889</v>
       </c>
       <c r="N15" s="60">
         <v>41926</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="O15" s="60">
+        <v>41939</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="59" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N16" s="60">
         <v>41926</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B17">
         <v>6</v>
       </c>
+      <c r="D17" s="62">
+        <v>0.67361111111111116</v>
+      </c>
       <c r="E17" s="1" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="J17" s="62">
+        <v>0.625</v>
       </c>
       <c r="N17" s="60">
         <v>41926</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="59" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B18">
         <v>7</v>
       </c>
+      <c r="D18" s="75">
+        <v>1.4444444444444444</v>
+      </c>
       <c r="E18" s="1" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N18" s="60">
         <v>41926</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="7"/>
-      <c r="N19" s="60"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+    <row r="19" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="D19" s="75">
+        <v>4.2152777777777777</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="N19" s="60">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="D20" s="75">
+        <v>4.1736111111111116</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="N20" s="60">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="D21" s="75">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J21" s="62">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="N21" s="60">
+        <v>41932</v>
+      </c>
+      <c r="O21" s="60">
+        <v>41939</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="D22" s="62">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="62">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="N22" s="60">
+        <v>41940</v>
+      </c>
+      <c r="O22" s="60">
+        <v>41956</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="D23" s="62">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="N23" s="60">
+        <v>41943</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="43"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7972,22 +8172,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -7998,7 +8198,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>1</v>
@@ -8034,7 +8234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -8053,7 +8253,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -8077,14 +8277,11 @@
       <c r="I3" s="4">
         <v>2</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
       <c r="M3" s="2"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -8108,15 +8305,13 @@
       <c r="I4" s="51">
         <v>1</v>
       </c>
-      <c r="J4" s="52">
-        <v>1.2</v>
-      </c>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
       <c r="M4" s="2"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -8140,15 +8335,13 @@
       <c r="I5" s="53">
         <v>1</v>
       </c>
-      <c r="J5" s="53">
-        <v>2</v>
-      </c>
+      <c r="J5" s="53"/>
       <c r="K5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="19"/>
       <c r="C6" s="6"/>
@@ -8163,7 +8356,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
@@ -8178,7 +8371,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>24</v>
       </c>
@@ -8197,71 +8390,130 @@
       <c r="N8" s="42"/>
       <c r="O8" s="43"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="C9" s="61"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="D9" s="62">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N9" s="60">
+        <v>41950</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
       <c r="C10" s="61"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="D10" s="62">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="N10" s="60">
+        <v>41955</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
       <c r="C11" s="61"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" s="62">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="N11" s="60">
+        <v>41956</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="C12" s="61"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="C13" s="61"/>
       <c r="G13" s="7"/>
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C14" s="61"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C15" s="61"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C16" s="61"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C17" s="61"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C18" s="61"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C19" s="61"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C20" s="61"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C21" s="61"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C22" s="61"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C23" s="61"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="45" t="s">
         <v>8</v>
       </c>
@@ -8293,18 +8545,18 @@
       <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -8351,7 +8603,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -8370,7 +8622,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -8401,7 +8653,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -8433,7 +8685,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -8465,7 +8717,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="19"/>
       <c r="C6" s="6"/>
@@ -8480,7 +8732,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
@@ -8495,7 +8747,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>24</v>
       </c>
@@ -8514,7 +8766,7 @@
       <c r="N8" s="42"/>
       <c r="O8" s="43"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="44" t="s">
         <v>23</v>
       </c>
@@ -8533,7 +8785,7 @@
       <c r="N17" s="42"/>
       <c r="O17" s="43"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="45" t="s">
         <v>8</v>
       </c>
@@ -8565,18 +8817,18 @@
       <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
@@ -8623,7 +8875,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -8642,7 +8894,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -8666,7 +8918,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -8692,7 +8944,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -8718,7 +8970,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
@@ -8735,7 +8987,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -8752,7 +9004,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
@@ -8769,7 +9021,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
@@ -8788,28 +9040,28 @@
       <c r="N9" s="42"/>
       <c r="O9" s="43"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O11" s="60"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O12" s="60"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O13" s="60"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O14" s="60"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O15" s="60"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O16" s="60"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O17" s="60"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="44" t="s">
         <v>23</v>
       </c>
@@ -8828,7 +9080,7 @@
       <c r="N18" s="42"/>
       <c r="O18" s="43"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
         <v>8</v>
       </c>
@@ -8853,18 +9105,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8982,14 +9234,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A72C14-AAB0-41A8-AF9B-22D04EB8DF14}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF3CF34B-E2F6-4638-94A3-0D272C4219B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -9000,6 +9244,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A72C14-AAB0-41A8-AF9B-22D04EB8DF14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>